<commit_message>
Exporting from MS SQL to MySQL use  SeedDataToMySql(); PLEASE
</commit_message>
<xml_diff>
--- a/DatabaseAppsProject/DatabaseApps.Client/Output-Files/Report.xlsx
+++ b/DatabaseAppsProject/DatabaseApps.Client/Output-Files/Report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Vendor</t>
   </si>
@@ -36,27 +36,6 @@
   </si>
   <si>
     <t>Targovishte Bottling Company Ltd.</t>
-  </si>
-  <si>
-    <t>Devin Bulgaria Ltd.</t>
-  </si>
-  <si>
-    <t>Coca-Cola Bg Corp.</t>
-  </si>
-  <si>
-    <t>Roi's Nuts Corp.</t>
-  </si>
-  <si>
-    <t>Jack Daniels Bulgaria Corp.</t>
-  </si>
-  <si>
-    <t>Chipi Chips Bulgaria Corp.</t>
-  </si>
-  <si>
-    <t>Orbit Bulgaria.</t>
-  </si>
-  <si>
-    <t>BulgarTabac Holding</t>
   </si>
 </sst>
 </file>
@@ -102,7 +81,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -130,16 +109,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="0">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="C2" s="0">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D2" s="0">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E2" s="0">
-        <v>0</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3">
@@ -147,16 +126,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="0">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C3" s="0">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="D3" s="0">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E3" s="0">
-        <v>0</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="4">
@@ -164,135 +143,118 @@
         <v>7</v>
       </c>
       <c r="B4" s="0">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C4" s="0">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D4" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E4" s="0">
-        <v>0</v>
+        <v>-125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" s="0">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="C5" s="0">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D5" s="0">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E5" s="0">
-        <v>0</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C6" s="0">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="D6" s="0">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E6" s="0">
-        <v>0</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" s="0">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C7" s="0">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D7" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E7" s="0">
-        <v>0</v>
+        <v>-125</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B8" s="0">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="C8" s="0">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D8" s="0">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E8" s="0">
-        <v>0</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B9" s="0">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C9" s="0">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="D9" s="0">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E9" s="0">
-        <v>0</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B10" s="0">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C10" s="0">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D10" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E10" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="0">
-        <v>0</v>
-      </c>
-      <c r="C11" s="0">
-        <v>0</v>
-      </c>
-      <c r="D11" s="0">
-        <v>0</v>
-      </c>
-      <c r="E11" s="0">
-        <v>0</v>
+        <v>-125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MySql fix for the new models. Minor fix on MySql db schema for more light data transfer.
</commit_message>
<xml_diff>
--- a/DatabaseAppsProject/DatabaseApps.Client/Output-Files/Report.xlsx
+++ b/DatabaseAppsProject/DatabaseApps.Client/Output-Files/Report.xlsx
@@ -81,7 +81,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -206,57 +206,6 @@
         <v>-125</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="0">
-        <v>200</v>
-      </c>
-      <c r="C8" s="0">
-        <v>30</v>
-      </c>
-      <c r="D8" s="0">
-        <v>36</v>
-      </c>
-      <c r="E8" s="0">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="0">
-        <v>100</v>
-      </c>
-      <c r="C9" s="0">
-        <v>120</v>
-      </c>
-      <c r="D9" s="0">
-        <v>20</v>
-      </c>
-      <c r="E9" s="0">
-        <v>-40</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="0">
-        <v>100</v>
-      </c>
-      <c r="C10" s="0">
-        <v>200</v>
-      </c>
-      <c r="D10" s="0">
-        <v>25</v>
-      </c>
-      <c r="E10" s="0">
-        <v>-125</v>
-      </c>
-    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
added the command interpretation engine.
</commit_message>
<xml_diff>
--- a/DatabaseAppsProject/DatabaseApps.Client/Output-Files/Report.xlsx
+++ b/DatabaseAppsProject/DatabaseApps.Client/Output-Files/Report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Vendor</t>
   </si>
@@ -36,6 +36,27 @@
   </si>
   <si>
     <t>Targovishte Bottling Company Ltd.</t>
+  </si>
+  <si>
+    <t>Devin Bulgaria Ltd.</t>
+  </si>
+  <si>
+    <t>Coca-Cola Bg Corp.</t>
+  </si>
+  <si>
+    <t>Roi's Nuts Corp.</t>
+  </si>
+  <si>
+    <t>Jack Daniels Bulgaria Corp.</t>
+  </si>
+  <si>
+    <t>Chipi Chips Bulgaria Corp.</t>
+  </si>
+  <si>
+    <t>Orbit Bulgaria.</t>
+  </si>
+  <si>
+    <t>BulgarTabac Holding</t>
   </si>
 </sst>
 </file>
@@ -81,7 +102,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -109,50 +130,50 @@
         <v>5</v>
       </c>
       <c r="B2" s="0">
-        <v>200</v>
+        <v>1736.34</v>
       </c>
       <c r="C2" s="0">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="D2" s="0">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0">
-        <v>134</v>
+        <v>1596.34</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D3" s="0">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E3" s="0">
-        <v>-40</v>
+        <v>-140</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C4" s="0">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="D4" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E4" s="0">
-        <v>-125</v>
+        <v>-140</v>
       </c>
     </row>
     <row r="5">
@@ -160,50 +181,288 @@
         <v>5</v>
       </c>
       <c r="B5" s="0">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="C5" s="0">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="D5" s="0">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E5" s="0">
-        <v>134</v>
+        <v>-140</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D6" s="0">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E6" s="0">
-        <v>-40</v>
+        <v>-140</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0">
+        <v>140</v>
+      </c>
+      <c r="D7" s="0">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0">
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="0">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0">
+        <v>140</v>
+      </c>
+      <c r="D8" s="0">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0">
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="0">
+        <v>3265.92</v>
+      </c>
+      <c r="C9" s="0">
+        <v>600</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0">
+        <v>2665.92</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="0">
+        <v>0</v>
+      </c>
+      <c r="C10" s="0">
+        <v>600</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0">
+        <v>-600</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0">
-        <v>100</v>
-      </c>
-      <c r="C7" s="0">
-        <v>200</v>
-      </c>
-      <c r="D7" s="0">
-        <v>25</v>
-      </c>
-      <c r="E7" s="0">
-        <v>-125</v>
+      <c r="B11" s="0">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0">
+        <v>760</v>
+      </c>
+      <c r="D11" s="0">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0">
+        <v>-760</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="0">
+        <v>0</v>
+      </c>
+      <c r="C12" s="0">
+        <v>760</v>
+      </c>
+      <c r="D12" s="0">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0">
+        <v>-760</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="0">
+        <v>0</v>
+      </c>
+      <c r="C13" s="0">
+        <v>760</v>
+      </c>
+      <c r="D13" s="0">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0">
+        <v>-760</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="0">
+        <v>0</v>
+      </c>
+      <c r="C14" s="0">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="0">
+        <v>0</v>
+      </c>
+      <c r="C15" s="0">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="0">
+        <v>0</v>
+      </c>
+      <c r="C16" s="0">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="0">
+        <v>0</v>
+      </c>
+      <c r="C17" s="0">
+        <v>0</v>
+      </c>
+      <c r="D17" s="0">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="0">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="0">
+        <v>0</v>
+      </c>
+      <c r="C19" s="0">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="0">
+        <v>0</v>
+      </c>
+      <c r="C20" s="0">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="0">
+        <v>0</v>
+      </c>
+      <c r="C21" s="0">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>